<commit_message>
update the molar volume calculations
</commit_message>
<xml_diff>
--- a/02_Dataset_EDA_Feature_UMAP_Mahalanobis/new FeCrNiCoV to corrosion dataset.xlsx
+++ b/02_Dataset_EDA_Feature_UMAP_Mahalanobis/new FeCrNiCoV to corrosion dataset.xlsx
@@ -684,10 +684,10 @@
         </is>
       </c>
       <c r="AE2" t="n">
-        <v>3.041907548904419</v>
+        <v>2.840407848358154</v>
       </c>
       <c r="AF2" t="n">
-        <v>11.68694877624512</v>
+        <v>12.974853515625</v>
       </c>
     </row>
     <row r="3">
@@ -784,10 +784,10 @@
         </is>
       </c>
       <c r="AE3" t="n">
-        <v>3.33547043800354</v>
+        <v>3.031013250350952</v>
       </c>
       <c r="AF3" t="n">
-        <v>11.42789173126221</v>
+        <v>12.57294654846191</v>
       </c>
     </row>
     <row r="4">
@@ -884,10 +884,10 @@
         </is>
       </c>
       <c r="AE4" t="n">
-        <v>3.478623628616333</v>
+        <v>3.167018413543701</v>
       </c>
       <c r="AF4" t="n">
-        <v>11.58323669433594</v>
+        <v>12.68288230895996</v>
       </c>
     </row>
     <row r="5">
@@ -984,10 +984,10 @@
         </is>
       </c>
       <c r="AE5" t="n">
-        <v>3.689864873886108</v>
+        <v>3.325519800186157</v>
       </c>
       <c r="AF5" t="n">
-        <v>11.60599803924561</v>
+        <v>12.58668422698975</v>
       </c>
     </row>
     <row r="6">
@@ -1084,10 +1084,10 @@
         </is>
       </c>
       <c r="AE6" t="n">
-        <v>3.751472473144531</v>
+        <v>3.4575035572052</v>
       </c>
       <c r="AF6" t="n">
-        <v>11.76002502441406</v>
+        <v>12.79450035095215</v>
       </c>
     </row>
     <row r="7">
@@ -1184,10 +1184,10 @@
         </is>
       </c>
       <c r="AE7" t="n">
-        <v>2.452622652053833</v>
+        <v>2.281842708587646</v>
       </c>
       <c r="AF7" t="n">
-        <v>11.37815475463867</v>
+        <v>12.56695747375488</v>
       </c>
     </row>
     <row r="8">
@@ -1284,10 +1284,10 @@
         </is>
       </c>
       <c r="AE8" t="n">
-        <v>2.792523860931396</v>
+        <v>2.592242479324341</v>
       </c>
       <c r="AF8" t="n">
-        <v>11.60393714904785</v>
+        <v>12.80287265777588</v>
       </c>
     </row>
     <row r="9">
@@ -1384,10 +1384,10 @@
         </is>
       </c>
       <c r="AE9" t="n">
-        <v>3.097952365875244</v>
+        <v>2.847051620483398</v>
       </c>
       <c r="AF9" t="n">
-        <v>11.61044025421143</v>
+        <v>12.79043388366699</v>
       </c>
     </row>
     <row r="10">
@@ -1484,10 +1484,10 @@
         </is>
       </c>
       <c r="AE10" t="n">
-        <v>3.390411853790283</v>
+        <v>3.142376661300659</v>
       </c>
       <c r="AF10" t="n">
-        <v>11.73797702789307</v>
+        <v>12.82507419586182</v>
       </c>
     </row>
     <row r="11">
@@ -1584,10 +1584,10 @@
         </is>
       </c>
       <c r="AE11" t="n">
-        <v>3.608765363693237</v>
+        <v>3.382583618164062</v>
       </c>
       <c r="AF11" t="n">
-        <v>11.66276359558105</v>
+        <v>12.70583057403564</v>
       </c>
     </row>
     <row r="12">
@@ -1684,10 +1684,10 @@
         </is>
       </c>
       <c r="AE12" t="n">
-        <v>3.929029226303101</v>
+        <v>3.685203790664673</v>
       </c>
       <c r="AF12" t="n">
-        <v>11.94819736480713</v>
+        <v>12.91453552246094</v>
       </c>
     </row>
     <row r="13">
@@ -1784,10 +1784,10 @@
         </is>
       </c>
       <c r="AE13" t="n">
-        <v>3.977468967437744</v>
+        <v>3.829819917678833</v>
       </c>
       <c r="AF13" t="n">
-        <v>12.28907871246338</v>
+        <v>13.22307395935059</v>
       </c>
     </row>
     <row r="14">
@@ -1884,10 +1884,10 @@
         </is>
       </c>
       <c r="AE14" t="n">
-        <v>1.337149024009705</v>
+        <v>1.420221567153931</v>
       </c>
       <c r="AF14" t="n">
-        <v>11.16105937957764</v>
+        <v>12.45138072967529</v>
       </c>
     </row>
     <row r="15">
@@ -1984,10 +1984,10 @@
         </is>
       </c>
       <c r="AE15" t="n">
-        <v>1.994356751441956</v>
+        <v>1.835132598876953</v>
       </c>
       <c r="AF15" t="n">
-        <v>11.4553337097168</v>
+        <v>12.84426498413086</v>
       </c>
     </row>
     <row r="16">
@@ -2084,10 +2084,10 @@
         </is>
       </c>
       <c r="AE16" t="n">
-        <v>2.516579866409302</v>
+        <v>2.31755518913269</v>
       </c>
       <c r="AF16" t="n">
-        <v>11.64659786224365</v>
+        <v>12.93618583679199</v>
       </c>
     </row>
     <row r="17">
@@ -2184,10 +2184,10 @@
         </is>
       </c>
       <c r="AE17" t="n">
-        <v>2.84837818145752</v>
+        <v>2.627319097518921</v>
       </c>
       <c r="AF17" t="n">
-        <v>11.79211902618408</v>
+        <v>12.97330188751221</v>
       </c>
     </row>
     <row r="18">
@@ -2284,10 +2284,10 @@
         </is>
       </c>
       <c r="AE18" t="n">
-        <v>3.069735765457153</v>
+        <v>2.817667961120605</v>
       </c>
       <c r="AF18" t="n">
-        <v>11.86001110076904</v>
+        <v>12.99754905700684</v>
       </c>
     </row>
     <row r="19">
@@ -2384,10 +2384,10 @@
         </is>
       </c>
       <c r="AE19" t="n">
-        <v>3.542096376419067</v>
+        <v>3.306522607803345</v>
       </c>
       <c r="AF19" t="n">
-        <v>11.91936683654785</v>
+        <v>12.9640417098999</v>
       </c>
     </row>
     <row r="20">
@@ -2484,10 +2484,10 @@
         </is>
       </c>
       <c r="AE20" t="n">
-        <v>3.778618812561035</v>
+        <v>3.604533195495605</v>
       </c>
       <c r="AF20" t="n">
-        <v>12.20728206634521</v>
+        <v>13.22229099273682</v>
       </c>
     </row>
     <row r="21">
@@ -2584,10 +2584,10 @@
         </is>
       </c>
       <c r="AE21" t="n">
-        <v>4.133970737457275</v>
+        <v>4.06130313873291</v>
       </c>
       <c r="AF21" t="n">
-        <v>12.5276403427124</v>
+        <v>13.41179466247559</v>
       </c>
     </row>
     <row r="22">
@@ -2684,10 +2684,10 @@
         </is>
       </c>
       <c r="AE22" t="n">
-        <v>4.21656608581543</v>
+        <v>4.217324256896973</v>
       </c>
       <c r="AF22" t="n">
-        <v>12.83265781402588</v>
+        <v>13.59045791625977</v>
       </c>
     </row>
     <row r="23">
@@ -2784,10 +2784,10 @@
         </is>
       </c>
       <c r="AE23" t="n">
-        <v>1.644803643226624</v>
+        <v>1.282296419143677</v>
       </c>
       <c r="AF23" t="n">
-        <v>11.55766773223877</v>
+        <v>13.28883266448975</v>
       </c>
     </row>
     <row r="24">
@@ -2884,10 +2884,10 @@
         </is>
       </c>
       <c r="AE24" t="n">
-        <v>1.786874771118164</v>
+        <v>1.533604502677917</v>
       </c>
       <c r="AF24" t="n">
-        <v>11.62817001342773</v>
+        <v>13.19435882568359</v>
       </c>
     </row>
     <row r="25">
@@ -2984,10 +2984,10 @@
         </is>
       </c>
       <c r="AE25" t="n">
-        <v>2.138756036758423</v>
+        <v>1.886880040168762</v>
       </c>
       <c r="AF25" t="n">
-        <v>11.52945804595947</v>
+        <v>13.02475070953369</v>
       </c>
     </row>
     <row r="26">
@@ -3084,10 +3084,10 @@
         </is>
       </c>
       <c r="AE26" t="n">
-        <v>2.461393594741821</v>
+        <v>2.233947038650513</v>
       </c>
       <c r="AF26" t="n">
-        <v>11.84250450134277</v>
+        <v>13.18631267547607</v>
       </c>
     </row>
     <row r="27">
@@ -3184,10 +3184,10 @@
         </is>
       </c>
       <c r="AE27" t="n">
-        <v>3.05091404914856</v>
+        <v>2.816362857818604</v>
       </c>
       <c r="AF27" t="n">
-        <v>11.99824142456055</v>
+        <v>13.17830085754395</v>
       </c>
     </row>
     <row r="28">
@@ -3284,10 +3284,10 @@
         </is>
       </c>
       <c r="AE28" t="n">
-        <v>3.432747602462769</v>
+        <v>3.263370513916016</v>
       </c>
       <c r="AF28" t="n">
-        <v>12.35552501678467</v>
+        <v>13.40875911712646</v>
       </c>
     </row>
     <row r="29">
@@ -3384,10 +3384,10 @@
         </is>
       </c>
       <c r="AE29" t="n">
-        <v>3.730124235153198</v>
+        <v>3.610644578933716</v>
       </c>
       <c r="AF29" t="n">
-        <v>12.50634670257568</v>
+        <v>13.49584865570068</v>
       </c>
     </row>
     <row r="30">
@@ -3484,10 +3484,10 @@
         </is>
       </c>
       <c r="AE30" t="n">
-        <v>4.148750782012939</v>
+        <v>4.176106929779053</v>
       </c>
       <c r="AF30" t="n">
-        <v>12.92832565307617</v>
+        <v>13.77007389068604</v>
       </c>
     </row>
     <row r="31">
@@ -3584,10 +3584,10 @@
         </is>
       </c>
       <c r="AE31" t="n">
-        <v>4.367891311645508</v>
+        <v>4.412979125976562</v>
       </c>
       <c r="AF31" t="n">
-        <v>12.9963903427124</v>
+        <v>13.80388832092285</v>
       </c>
     </row>
     <row r="32">
@@ -3684,10 +3684,10 @@
         </is>
       </c>
       <c r="AE32" t="n">
-        <v>1.624837160110474</v>
+        <v>1.026296854019165</v>
       </c>
       <c r="AF32" t="n">
-        <v>11.70381927490234</v>
+        <v>13.68306922912598</v>
       </c>
     </row>
     <row r="33">
@@ -3784,10 +3784,10 @@
         </is>
       </c>
       <c r="AE33" t="n">
-        <v>1.773285269737244</v>
+        <v>1.280116200447083</v>
       </c>
       <c r="AF33" t="n">
-        <v>11.823899269104</v>
+        <v>13.55428123474121</v>
       </c>
     </row>
     <row r="34">
@@ -3884,10 +3884,10 @@
         </is>
       </c>
       <c r="AE34" t="n">
-        <v>1.935367584228516</v>
+        <v>1.588118433952332</v>
       </c>
       <c r="AF34" t="n">
-        <v>11.89328670501709</v>
+        <v>13.43269157409668</v>
       </c>
     </row>
     <row r="35">
@@ -3984,10 +3984,10 @@
         </is>
       </c>
       <c r="AE35" t="n">
-        <v>2.349958419799805</v>
+        <v>2.036976337432861</v>
       </c>
       <c r="AF35" t="n">
-        <v>11.95706939697266</v>
+        <v>13.32980155944824</v>
       </c>
     </row>
     <row r="36">
@@ -4084,10 +4084,10 @@
         </is>
       </c>
       <c r="AE36" t="n">
-        <v>2.813989162445068</v>
+        <v>2.535278797149658</v>
       </c>
       <c r="AF36" t="n">
-        <v>12.09293937683105</v>
+        <v>13.33436107635498</v>
       </c>
     </row>
     <row r="37">
@@ -4184,10 +4184,10 @@
         </is>
       </c>
       <c r="AE37" t="n">
-        <v>3.223434925079346</v>
+        <v>3.069841384887695</v>
       </c>
       <c r="AF37" t="n">
-        <v>12.49896812438965</v>
+        <v>13.60497093200684</v>
       </c>
     </row>
     <row r="38">
@@ -4284,10 +4284,10 @@
         </is>
       </c>
       <c r="AE38" t="n">
-        <v>3.749391555786133</v>
+        <v>3.69943642616272</v>
       </c>
       <c r="AF38" t="n">
-        <v>12.86458110809326</v>
+        <v>13.80571460723877</v>
       </c>
     </row>
     <row r="39">
@@ -4384,10 +4384,10 @@
         </is>
       </c>
       <c r="AE39" t="n">
-        <v>4.186276435852051</v>
+        <v>4.202789306640625</v>
       </c>
       <c r="AF39" t="n">
-        <v>13.0621395111084</v>
+        <v>13.82440662384033</v>
       </c>
     </row>
     <row r="40">
@@ -4484,10 +4484,10 @@
         </is>
       </c>
       <c r="AE40" t="n">
-        <v>4.423818588256836</v>
+        <v>4.484659671783447</v>
       </c>
       <c r="AF40" t="n">
-        <v>13.00998401641846</v>
+        <v>13.87829399108887</v>
       </c>
     </row>
     <row r="41">
@@ -4584,10 +4584,10 @@
         </is>
       </c>
       <c r="AE41" t="n">
-        <v>2.162084341049194</v>
+        <v>0.5137186646461487</v>
       </c>
       <c r="AF41" t="n">
-        <v>11.06163692474365</v>
+        <v>13.91857719421387</v>
       </c>
     </row>
     <row r="42">
@@ -4684,10 +4684,10 @@
         </is>
       </c>
       <c r="AE42" t="n">
-        <v>1.670606136322021</v>
+        <v>1.213401317596436</v>
       </c>
       <c r="AF42" t="n">
-        <v>12.07521724700928</v>
+        <v>13.89088344573975</v>
       </c>
     </row>
     <row r="43">
@@ -4784,10 +4784,10 @@
         </is>
       </c>
       <c r="AE43" t="n">
-        <v>1.782967567443848</v>
+        <v>1.401995062828064</v>
       </c>
       <c r="AF43" t="n">
-        <v>12.12575817108154</v>
+        <v>13.74648761749268</v>
       </c>
     </row>
     <row r="44">
@@ -4884,10 +4884,10 @@
         </is>
       </c>
       <c r="AE44" t="n">
-        <v>2.284972190856934</v>
+        <v>2.001736879348755</v>
       </c>
       <c r="AF44" t="n">
-        <v>12.35530757904053</v>
+        <v>13.81153774261475</v>
       </c>
     </row>
     <row r="45">
@@ -4984,10 +4984,10 @@
         </is>
       </c>
       <c r="AE45" t="n">
-        <v>2.75108814239502</v>
+        <v>2.496543169021606</v>
       </c>
       <c r="AF45" t="n">
-        <v>12.46909523010254</v>
+        <v>13.73969841003418</v>
       </c>
     </row>
     <row r="46">
@@ -5084,10 +5084,10 @@
         </is>
       </c>
       <c r="AE46" t="n">
-        <v>3.23347806930542</v>
+        <v>3.128198862075806</v>
       </c>
       <c r="AF46" t="n">
-        <v>12.72739028930664</v>
+        <v>13.81718349456787</v>
       </c>
     </row>
     <row r="47">
@@ -5184,10 +5184,10 @@
         </is>
       </c>
       <c r="AE47" t="n">
-        <v>3.524228811264038</v>
+        <v>3.537582159042358</v>
       </c>
       <c r="AF47" t="n">
-        <v>12.9974308013916</v>
+        <v>13.97863960266113</v>
       </c>
     </row>
     <row r="48">
@@ -5284,10 +5284,10 @@
         </is>
       </c>
       <c r="AE48" t="n">
-        <v>4.068644046783447</v>
+        <v>4.129258632659912</v>
       </c>
       <c r="AF48" t="n">
-        <v>13.20846939086914</v>
+        <v>14.03242778778076</v>
       </c>
     </row>
     <row r="49">
@@ -5384,10 +5384,10 @@
         </is>
       </c>
       <c r="AE49" t="n">
-        <v>4.320101737976074</v>
+        <v>4.395395278930664</v>
       </c>
       <c r="AF49" t="n">
-        <v>13.17461681365967</v>
+        <v>13.9338321685791</v>
       </c>
     </row>
     <row r="50">
@@ -5484,10 +5484,10 @@
         </is>
       </c>
       <c r="AE50" t="n">
-        <v>1.678680300712585</v>
+        <v>1.137687921524048</v>
       </c>
       <c r="AF50" t="n">
-        <v>12.26272678375244</v>
+        <v>14.14419078826904</v>
       </c>
     </row>
     <row r="51">
@@ -5584,10 +5584,10 @@
         </is>
       </c>
       <c r="AE51" t="n">
-        <v>1.584185361862183</v>
+        <v>1.28240966796875</v>
       </c>
       <c r="AF51" t="n">
-        <v>12.14484596252441</v>
+        <v>13.869140625</v>
       </c>
     </row>
     <row r="52">
@@ -5684,10 +5684,10 @@
         </is>
       </c>
       <c r="AE52" t="n">
-        <v>1.83100152015686</v>
+        <v>1.502074241638184</v>
       </c>
       <c r="AF52" t="n">
-        <v>12.48001861572266</v>
+        <v>14.07583332061768</v>
       </c>
     </row>
     <row r="53">
@@ -5784,10 +5784,10 @@
         </is>
       </c>
       <c r="AE53" t="n">
-        <v>2.24833869934082</v>
+        <v>2.02942967414856</v>
       </c>
       <c r="AF53" t="n">
-        <v>12.62903022766113</v>
+        <v>14.04880714416504</v>
       </c>
     </row>
     <row r="54">
@@ -5884,10 +5884,10 @@
         </is>
       </c>
       <c r="AE54" t="n">
-        <v>2.582781791687012</v>
+        <v>2.383607387542725</v>
       </c>
       <c r="AF54" t="n">
-        <v>12.631667137146</v>
+        <v>13.95694065093994</v>
       </c>
     </row>
     <row r="55">
@@ -5984,10 +5984,10 @@
         </is>
       </c>
       <c r="AE55" t="n">
-        <v>3.010164499282837</v>
+        <v>2.923919916152954</v>
       </c>
       <c r="AF55" t="n">
-        <v>12.86608409881592</v>
+        <v>13.96650886535645</v>
       </c>
     </row>
     <row r="56">
@@ -6084,10 +6084,10 @@
         </is>
       </c>
       <c r="AE56" t="n">
-        <v>3.558807134628296</v>
+        <v>3.538928985595703</v>
       </c>
       <c r="AF56" t="n">
-        <v>13.10269832611084</v>
+        <v>14.06075477600098</v>
       </c>
     </row>
     <row r="57">
@@ -6184,10 +6184,10 @@
         </is>
       </c>
       <c r="AE57" t="n">
-        <v>3.950931787490845</v>
+        <v>4.00605297088623</v>
       </c>
       <c r="AF57" t="n">
-        <v>13.2910737991333</v>
+        <v>14.11138916015625</v>
       </c>
     </row>
     <row r="58">
@@ -6284,10 +6284,10 @@
         </is>
       </c>
       <c r="AE58" t="n">
-        <v>4.260393619537354</v>
+        <v>4.343692779541016</v>
       </c>
       <c r="AF58" t="n">
-        <v>13.15990352630615</v>
+        <v>13.91593360900879</v>
       </c>
     </row>
     <row r="59">
@@ -6384,10 +6384,10 @@
         </is>
       </c>
       <c r="AE59" t="n">
-        <v>1.717764258384705</v>
+        <v>1.568461537361145</v>
       </c>
       <c r="AF59" t="n">
-        <v>12.77111434936523</v>
+        <v>14.43152809143066</v>
       </c>
     </row>
     <row r="60">
@@ -6484,10 +6484,10 @@
         </is>
       </c>
       <c r="AE60" t="n">
-        <v>1.845646739006042</v>
+        <v>1.712540864944458</v>
       </c>
       <c r="AF60" t="n">
-        <v>12.82676982879639</v>
+        <v>14.28320407867432</v>
       </c>
     </row>
     <row r="61">
@@ -6584,10 +6584,10 @@
         </is>
       </c>
       <c r="AE61" t="n">
-        <v>1.959308624267578</v>
+        <v>1.909233689308167</v>
       </c>
       <c r="AF61" t="n">
-        <v>12.91557312011719</v>
+        <v>14.4071159362793</v>
       </c>
     </row>
     <row r="62">
@@ -6684,10 +6684,10 @@
         </is>
       </c>
       <c r="AE62" t="n">
-        <v>2.35932183265686</v>
+        <v>2.268156290054321</v>
       </c>
       <c r="AF62" t="n">
-        <v>12.95022487640381</v>
+        <v>14.25215816497803</v>
       </c>
     </row>
     <row r="63">
@@ -6784,10 +6784,10 @@
         </is>
       </c>
       <c r="AE63" t="n">
-        <v>2.789191007614136</v>
+        <v>2.72359561920166</v>
       </c>
       <c r="AF63" t="n">
-        <v>13.02880668640137</v>
+        <v>14.18868160247803</v>
       </c>
     </row>
     <row r="64">
@@ -6884,10 +6884,10 @@
         </is>
       </c>
       <c r="AE64" t="n">
-        <v>3.359243154525757</v>
+        <v>3.324115991592407</v>
       </c>
       <c r="AF64" t="n">
-        <v>13.09835052490234</v>
+        <v>14.13976860046387</v>
       </c>
     </row>
     <row r="65">
@@ -6984,10 +6984,10 @@
         </is>
       </c>
       <c r="AE65" t="n">
-        <v>3.896231651306152</v>
+        <v>3.923548221588135</v>
       </c>
       <c r="AF65" t="n">
-        <v>13.19523620605469</v>
+        <v>14.05698585510254</v>
       </c>
     </row>
     <row r="66">
@@ -7084,10 +7084,10 @@
         </is>
       </c>
       <c r="AE66" t="n">
-        <v>1.919947385787964</v>
+        <v>1.746564507484436</v>
       </c>
       <c r="AF66" t="n">
-        <v>13.02512168884277</v>
+        <v>14.54662990570068</v>
       </c>
     </row>
     <row r="67">
@@ -7184,10 +7184,10 @@
         </is>
       </c>
       <c r="AE67" t="n">
-        <v>2.127997636795044</v>
+        <v>2.034261226654053</v>
       </c>
       <c r="AF67" t="n">
-        <v>12.95474147796631</v>
+        <v>14.33198738098145</v>
       </c>
     </row>
     <row r="68">
@@ -7284,10 +7284,10 @@
         </is>
       </c>
       <c r="AE68" t="n">
-        <v>2.404359102249146</v>
+        <v>2.308255910873413</v>
       </c>
       <c r="AF68" t="n">
-        <v>12.85120868682861</v>
+        <v>14.19418621063232</v>
       </c>
     </row>
     <row r="69">
@@ -7384,10 +7384,10 @@
         </is>
       </c>
       <c r="AE69" t="n">
-        <v>2.604987144470215</v>
+        <v>2.591636180877686</v>
       </c>
       <c r="AF69" t="n">
-        <v>13.16816806793213</v>
+        <v>14.37798118591309</v>
       </c>
     </row>
     <row r="70">
@@ -7484,10 +7484,10 @@
         </is>
       </c>
       <c r="AE70" t="n">
-        <v>3.221719026565552</v>
+        <v>3.16672158241272</v>
       </c>
       <c r="AF70" t="n">
-        <v>13.03928565979004</v>
+        <v>14.07291889190674</v>
       </c>
     </row>
   </sheetData>

</xml_diff>